<commit_message>
Kicad CAD for mainboard and motorboard (final)
</commit_message>
<xml_diff>
--- a/CAD/electrical/main_board_v2/bom.xlsx
+++ b/CAD/electrical/main_board_v2/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">100n capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C4,C12,C13,C14,C203,C206,C301</t>
+    <t xml:space="preserve">C2,C4,C12,C13,C14,C203,C206,C301</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor_SMD:C_0805_2012Metric</t>
@@ -46,6 +46,30 @@
     <t xml:space="preserve">C28233</t>
   </si>
   <si>
+    <t xml:space="preserve">100u capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1,C201,C202,C205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:CP_Elec_8x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C294509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000u capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:CP_Elec_10x10.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C336751</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED</t>
   </si>
   <si>
@@ -121,13 +145,22 @@
     <t xml:space="preserve">100u inductor</t>
   </si>
   <si>
+    <t xml:space="preserve">L201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor_SMD:L_12x12mm_H6mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C169378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10u inductor</t>
+  </si>
+  <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
-    <t xml:space="preserve">Inductor_SMD:L_12x12mm_H6mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C169378</t>
+    <t xml:space="preserve">C9904</t>
   </si>
   <si>
     <t xml:space="preserve">Basic NPN</t>
@@ -139,16 +172,16 @@
     <t xml:space="preserve">C20526</t>
   </si>
   <si>
-    <t xml:space="preserve">300 resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1,R4,R201,R202</t>
+    <t xml:space="preserve">470 resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R4,R201,R202,R9,R10,R14</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor_SMD:R_1206_3216Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">C17887</t>
+    <t xml:space="preserve">C23179</t>
   </si>
   <si>
     <t xml:space="preserve">33k resistor</t>
@@ -163,15 +196,6 @@
     <t xml:space="preserve">C4216</t>
   </si>
   <si>
-    <t xml:space="preserve">620 resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9,R10,R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23220</t>
-  </si>
-  <si>
     <t xml:space="preserve">10k resistor</t>
   </si>
   <si>
@@ -190,13 +214,13 @@
     <t xml:space="preserve">C23254</t>
   </si>
   <si>
-    <t xml:space="preserve">36k resistor</t>
+    <t xml:space="preserve">47k resistor</t>
   </si>
   <si>
     <t xml:space="preserve">R302</t>
   </si>
   <si>
-    <t xml:space="preserve">C23147</t>
+    <t xml:space="preserve">C25819</t>
   </si>
   <si>
     <t xml:space="preserve">100 resistor</t>
@@ -208,6 +232,12 @@
     <t xml:space="preserve">C22775</t>
   </si>
   <si>
+    <t xml:space="preserve">1k resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2,R3</t>
+  </si>
+  <si>
     <t xml:space="preserve">PCA9306DC</t>
   </si>
   <si>
@@ -278,6 +308,18 @@
   </si>
   <si>
     <t xml:space="preserve">C6568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2kO potentiometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentiometer_SMD:Potentiometer_Bourns_3314J_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C94513</t>
   </si>
 </sst>
 </file>
@@ -352,13 +394,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -378,350 +428,406 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>58</v>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="D22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="D23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="0" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>